<commit_message>
feat: implement the method to fit the observed data
Implement the KWFTree class that fits the data to produce the forward curve.
Include a method to retrieve the short rate curve from the adjusted forward
rate curve. Move the old library to 'old_trees.py'.
</commit_message>
<xml_diff>
--- a/KWF_model.xlsx
+++ b/KWF_model.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ucaiado/Temp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ucaiado/GIT/ShortRate_Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20180" windowHeight="21600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -120,8 +120,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
-    <numFmt numFmtId="172" formatCode="0.0000"/>
-    <numFmt numFmtId="173" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -279,18 +279,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="173" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="34">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -336,6 +336,951 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$81:$O$81</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.0349999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0423514965946841</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0506919725101942</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$82:$O$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.0349999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0423514965946841</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0466580607843014</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$83:$O$83</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.0349999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0378640974890103</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0436519418204204</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$84:$O$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.0349999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0378640974890103</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0403355037668061</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2146982752"/>
+        <c:axId val="-2146770176"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2146982752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2146770176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2146770176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.032"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2146982752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -601,10 +1546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I118"/>
+  <dimension ref="A1:P118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E3" sqref="E3:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -941,27 +1886,31 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H49" s="6"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F51" s="11">
         <f>((H47+H48)/(1+F53/100)+(H55+H56)/(1+F53/100))*0.5</f>
         <v>97.885516442585612</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F52" s="8">
         <v>4.5</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F53" s="9">
         <f>F61*EXP(2*_vol)</f>
         <v>6.7573669709288327</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="P53">
+        <f>1+F53/100</f>
+        <v>1.0675736697092884</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D55" s="11">
         <f>((F51+F52)/(1+D57/100)+(F59+F60)/(1+D57/100))*0.5</f>
         <v>98.073901662547669</v>
@@ -970,7 +1919,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D56" s="8">
         <v>4.5</v>
       </c>
@@ -978,19 +1927,23 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D57" s="9">
         <f>D65*EXP(2*_vol)</f>
         <v>4.9755210099688831</v>
       </c>
       <c r="H57" s="6"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="N57">
+        <f>1+D57/100</f>
+        <v>1.0497552100996888</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B58" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>12</v>
       </c>
@@ -1003,7 +1956,7 @@
         <v>99.021662047542279</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>11</v>
       </c>
@@ -1014,7 +1967,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>13</v>
       </c>
@@ -1025,8 +1978,16 @@
         <f>F69*EXP(2*_vol)</f>
         <v>5.5324641489328439</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M61" s="19">
+        <f>B61/100+1</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="P61">
+        <f>1+F61/100</f>
+        <v>1.0553246414893285</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D63" s="11">
         <f>((F59+F60)/(1+D65/100)+(F67+F68)/(1+D65/100))*0.5</f>
         <v>99.926072509206676</v>
@@ -1035,7 +1996,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D64" s="8">
         <v>4.5</v>
       </c>
@@ -1043,7 +2004,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -1054,37 +2015,123 @@
         <v>4.0736120634471442</v>
       </c>
       <c r="H65" s="6"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="N65">
+        <f>1+D65/100</f>
+        <v>1.0407361206344714</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F67" s="11">
         <f>((H63+H64)/(1+F69/100)+(H71+H72)/(1+F69/100))*0.5</f>
         <v>99.971684059399053</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F68" s="8">
         <v>4.5</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F69" s="10">
         <v>4.5295985390327234</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="P69">
+        <f>1+F69/100</f>
+        <v>1.0452959853903272</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H71" s="15">
         <v>100</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M71" s="19">
+        <f>M61</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="N71">
+        <f>N57*M71</f>
+        <v>1.0864966424531777</v>
+      </c>
+      <c r="O71">
+        <f>N71*P53</f>
+        <v>1.1599152077105594</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H72" s="16">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M72" s="19">
+        <f>M71</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="N72">
+        <f>N71</f>
+        <v>1.0864966424531777</v>
+      </c>
+      <c r="O72">
+        <f>N72*P61</f>
+        <v>1.1466066796762588</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H73" s="17"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M73" s="19">
+        <f>M72</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="N73">
+        <f>N65*M73</f>
+        <v>1.0771618848566777</v>
+      </c>
+      <c r="O73">
+        <f>N73*P61</f>
+        <v>1.1367554799623427</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M74" s="19">
+        <f>M73</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="N74">
+        <f>N73</f>
+        <v>1.0771618848566777</v>
+      </c>
+      <c r="O74">
+        <f>N74*P69</f>
+        <v>1.1259529938561632</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M76">
+        <f>M71^(1/1)</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="N76">
+        <f>N71^(1/2)</f>
+        <v>1.0423514965946841</v>
+      </c>
+      <c r="O76">
+        <f>O71^(1/3)</f>
+        <v>1.0506919725101942</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M77">
+        <f t="shared" ref="M77:M79" si="0">M72^(1/1)</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="N77">
+        <f t="shared" ref="N77:N79" si="1">N72^(1/2)</f>
+        <v>1.0423514965946841</v>
+      </c>
+      <c r="O77">
+        <f t="shared" ref="O77:O79" si="2">O72^(1/3)</f>
+        <v>1.0466580607843015</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B78" s="19">
         <f>B61</f>
         <v>3.5</v>
@@ -1097,8 +2144,20 @@
         <f>(F69+F61+F53)/3</f>
         <v>5.6064765529648</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M78">
+        <f t="shared" si="0"/>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="N78">
+        <f t="shared" si="1"/>
+        <v>1.0378640974890103</v>
+      </c>
+      <c r="O78">
+        <f t="shared" si="2"/>
+        <v>1.0436519418204204</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B79">
         <f>1+B78/100</f>
         <v>1.0349999999999999</v>
@@ -1111,8 +2170,20 @@
         <f>1+F78/100</f>
         <v>1.056064765529648</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M79">
+        <f t="shared" si="0"/>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="N79">
+        <f t="shared" si="1"/>
+        <v>1.0378640974890103</v>
+      </c>
+      <c r="O79">
+        <f t="shared" si="2"/>
+        <v>1.0403355037668061</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>23</v>
       </c>
@@ -1131,25 +2202,95 @@
         <v>4.5401436899321412E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M81">
+        <f>M76-1</f>
+        <v>3.499999999999992E-2</v>
+      </c>
+      <c r="N81">
+        <f t="shared" ref="N81:O81" si="3">N76-1</f>
+        <v>4.2351496594684068E-2</v>
+      </c>
+      <c r="O81">
+        <f t="shared" si="3"/>
+        <v>5.0691972510194194E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M82">
+        <f t="shared" ref="M82:O82" si="4">M77-1</f>
+        <v>3.499999999999992E-2</v>
+      </c>
+      <c r="N82">
+        <f t="shared" si="4"/>
+        <v>4.2351496594684068E-2</v>
+      </c>
+      <c r="O82">
+        <f t="shared" si="4"/>
+        <v>4.6658060784301458E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M83">
+        <f t="shared" ref="M83:O83" si="5">M78-1</f>
+        <v>3.499999999999992E-2</v>
+      </c>
+      <c r="N83">
+        <f t="shared" si="5"/>
+        <v>3.7864097489010318E-2</v>
+      </c>
+      <c r="O83">
+        <f t="shared" si="5"/>
+        <v>4.3651941820420426E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M84">
+        <f t="shared" ref="M84:O84" si="6">M79-1</f>
+        <v>3.499999999999992E-2</v>
+      </c>
+      <c r="N84">
+        <f t="shared" si="6"/>
+        <v>3.7864097489010318E-2</v>
+      </c>
+      <c r="O84">
+        <f t="shared" si="6"/>
+        <v>4.0335503766806058E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M86">
+        <f>AVERAGE(M81:M84)</f>
+        <v>3.499999999999992E-2</v>
+      </c>
+      <c r="N86">
+        <f>AVERAGE(N81:N84)</f>
+        <v>4.0107797041847193E-2</v>
+      </c>
+      <c r="O86">
+        <f>AVERAGE(O81:O84)</f>
+        <v>4.5334369720430534E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="H92" s="7">
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="H93" s="18">
         <v>5.25</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="H94" s="6"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F96" s="11">
         <f>((H92+H93)/(1+F98/100)+(H100+H101)/(1+F98/100))*0.5</f>
         <v>98.588044072556315</v>
@@ -1295,5 +2436,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>